<commit_message>
Adicionei métricas do selection sort
</commit_message>
<xml_diff>
--- a/Medidas.xlsx
+++ b/Medidas.xlsx
@@ -8,28 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b11f3926168ae189/Área de Trabalho/ED/Algoritmos-de-Ordenacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{82FD250B-5291-481F-82C3-57C288BC4F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C62D36C8-240B-457F-B6C9-84F6DCE69AF1}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{82FD250B-5291-481F-82C3-57C288BC4F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{870C2A26-0398-4546-9730-CA864BC1FB42}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{040B720E-10F0-4BD9-9CC3-7F59FC5AA694}"/>
   </bookViews>
   <sheets>
     <sheet name="Bubble Sort" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Selection Sort" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Bubble Sort'!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Bubble Sort'!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Bubble Sort'!$B$2:$B$26</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Bubble Sort'!$C$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Bubble Sort'!$C$2:$C$26</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Selection Sort'!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Selection Sort'!$C$2:$C$51</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Bubble Sort'!$C$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Bubble Sort'!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Bubble Sort'!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Bubble Sort'!$B$2:$B$51</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Bubble Sort'!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Bubble Sort'!$C$2:$C$51</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Bubble Sort'!#REF!</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Bubble Sort'!$B$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Selection Sort'!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Selection Sort'!$B$2:$B$51</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Selection Sort'!$C$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Selection Sort'!$C$2:$C$51</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Selection Sort'!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Selection Sort'!$B$2:$B$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Normal</t>
   </si>
@@ -88,6 +87,12 @@
   </si>
   <si>
     <t>Bubble Sort Otimizado</t>
+  </si>
+  <si>
+    <t>Selection Sort Normal</t>
+  </si>
+  <si>
+    <t>Selection Sort Otimizado</t>
   </si>
 </sst>
 </file>
@@ -147,12 +152,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -190,7 +195,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B3973A66-B310-47D9-90FC-CCE90989F831}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Bubble Sort Normal</cx:v>
             </cx:txData>
           </cx:tx>
@@ -203,7 +208,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{457C901A-BD39-46C9-AA69-C923AEEE3817}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Bubble Sort Otimizado</cx:v>
             </cx:txData>
           </cx:tx>
@@ -214,13 +219,100 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
+      <cx:axis id="0" hidden="1">
         <cx:catScaling gapWidth="1"/>
         <cx:tickLabels/>
         <cx:numFmt formatCode="Geral" sourceLinked="0"/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling max="1300000000" min="600000000"/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribuição dos tempos</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            </a:rPr>
+            <a:t>Distribuição dos tempos</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{B3973A66-B310-47D9-90FC-CCE90989F831}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v>Selection Sort Normal</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{457C901A-BD39-46C9-AA69-C923AEEE3817}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>Selection Sort Otimizado</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="Geral" sourceLinked="0"/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="900000000" min="300000000"/>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -269,7 +361,562 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -833,8 +1480,91 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2532784" y="126422"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="4041198" y="126422"/>
+              <a:ext cx="4595899" cy="2758786"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Este gráfico não está disponível na sua versão de Excel.
+Editar esta forma ou salvar esta pasta de trabalho em um formato de arquivo diferente quebrará o gráfico permanentemente.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>688398</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>126422</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>316057</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142008</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82328681-FC67-451D-B8AD-3CC5CA7B9A05}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4041198" y="126422"/>
+              <a:ext cx="4595899" cy="2758786"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -876,6 +1606,18 @@
     <tableColumn id="3" xr3:uid="{6A0AF59B-3895-47C2-B3F1-A66C304DC4FE}" name="Bubble Sort Otimizado"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{29EF381D-2F20-47A8-899F-A5B7194C3D74}" name="Tabela13" displayName="Tabela13" ref="A1:C51" totalsRowShown="0">
+  <autoFilter ref="A1:C51" xr:uid="{D7C597AC-17F2-4DE2-87F8-9C442AE8B236}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6FB3F639-B5B9-494E-836C-5FA1EE0D68C8}" name="Seed"/>
+    <tableColumn id="2" xr3:uid="{98A5E298-86D0-480B-AD3B-6C5E05874EA5}" name="Selection Sort Normal"/>
+    <tableColumn id="3" xr3:uid="{2891C752-66A8-46F5-863D-C345D75AEBB5}" name="Selection Sort Otimizado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1199,7 +1941,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1867,220 +2609,674 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1573F65-7B1F-412B-A120-DD6344D9F4D4}">
-  <dimension ref="B2:C26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767D3CC7-47F0-4937-A42E-6FF70D3BDA26}">
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F51"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>325415100</v>
+        <v>596788400</v>
       </c>
       <c r="C2">
-        <v>294653300</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>393076200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3">
-        <v>417680200</v>
+        <v>598705100</v>
       </c>
       <c r="C3">
-        <v>342644300</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+        <v>351998000</v>
+      </c>
+      <c r="P3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4">
-        <v>359141600</v>
+        <v>731019400</v>
       </c>
       <c r="C4">
-        <v>343493700</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+        <v>436639500</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <f>AVERAGE(B2:B51)</f>
+        <v>741806638</v>
+      </c>
+      <c r="Q4">
+        <f>AVERAGE(C2:C51)</f>
+        <v>425489066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5">
-        <v>335553800</v>
+        <v>708295300</v>
       </c>
       <c r="C5">
-        <v>292277300</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+        <v>432021700</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <f>_xlfn.STDEV.S(B2:B51)</f>
+        <v>49011545.332036175</v>
+      </c>
+      <c r="Q5">
+        <f>_xlfn.STDEV.S(C2:C51)</f>
+        <v>26833741.57417554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6">
-        <v>299212600</v>
+        <v>744140500</v>
       </c>
       <c r="C6">
-        <v>297845600</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+        <v>408164200</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <f>MIN(B2:B51)</f>
+        <v>596788400</v>
+      </c>
+      <c r="Q6">
+        <f>MIN(C2:C51)</f>
+        <v>351998000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="B7">
-        <v>326159800</v>
+        <v>769097000</v>
       </c>
       <c r="C7">
-        <v>307199300</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+        <v>435484600</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <f>_xlfn.QUARTILE.EXC(B2:B51,1)</f>
+        <v>711577350</v>
+      </c>
+      <c r="Q7">
+        <f>_xlfn.QUARTILE.EXC(C2:C51,1)</f>
+        <v>403868075</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8">
-        <v>348131000</v>
+        <v>682787900</v>
       </c>
       <c r="C8">
-        <v>348567500</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+        <v>421828300</v>
+      </c>
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <f>_xlfn.QUARTILE.EXC(B2:B51,2)</f>
+        <v>744035950</v>
+      </c>
+      <c r="Q8">
+        <f>_xlfn.QUARTILE.EXC(C2:C51,2)</f>
+        <v>430140650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9">
-        <v>338434800</v>
+        <v>805348500</v>
       </c>
       <c r="C9">
-        <v>311045200</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+        <v>435312400</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <f>_xlfn.QUARTILE.EXC(B2:B51,3)</f>
+        <v>772217075</v>
+      </c>
+      <c r="Q9">
+        <f>_xlfn.QUARTILE.EXC(C2:C51,3)</f>
+        <v>444680900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10">
-        <v>323796300</v>
+        <v>799131000</v>
       </c>
       <c r="C10">
-        <v>321567300</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+        <v>413124700</v>
+      </c>
+      <c r="O10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <f>MAX(B2:B51)</f>
+        <v>848884600</v>
+      </c>
+      <c r="Q10">
+        <f>MAX(C2:C51)</f>
+        <v>488389400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11">
-        <v>300929700</v>
+        <v>729613100</v>
       </c>
       <c r="C11">
-        <v>326196200</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+        <v>434996900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12">
-        <v>362400900</v>
+        <v>707999800</v>
       </c>
       <c r="C12">
-        <v>348997000</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+        <v>393873400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13">
-        <v>318908600</v>
+        <v>750292500</v>
       </c>
       <c r="C13">
-        <v>355481800</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+        <v>394780200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14">
-        <v>1586590100</v>
+        <v>689056900</v>
       </c>
       <c r="C14">
-        <v>325054400</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+        <v>468335700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15">
-        <v>1727691100</v>
+        <v>746109800</v>
       </c>
       <c r="C15">
-        <v>342067300</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+        <v>404691800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16">
-        <v>1514647200</v>
+        <v>722693700</v>
       </c>
       <c r="C16">
-        <v>325474000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+        <v>424948500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17">
-        <v>1470438500</v>
+        <v>708960000</v>
       </c>
       <c r="C17">
-        <v>343286500</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+        <v>387263200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18">
-        <v>1561448700</v>
+        <v>765166700</v>
       </c>
       <c r="C18">
-        <v>316192900</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+        <v>454179800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19">
-        <v>1612642700</v>
+        <v>756450000</v>
       </c>
       <c r="C19">
-        <v>305103800</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+        <v>452025800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20">
-        <v>1464116500</v>
+        <v>750644300</v>
       </c>
       <c r="C20">
-        <v>292193700</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+        <v>452450800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21">
-        <v>1753291700</v>
+        <v>759764200</v>
       </c>
       <c r="C21">
-        <v>322189600</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+        <v>381811800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22">
-        <v>1771767500</v>
+        <v>706919500</v>
       </c>
       <c r="C22">
-        <v>291903700</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+        <v>449231400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23">
-        <v>1670596000</v>
+        <v>715342800</v>
       </c>
       <c r="C23">
-        <v>291530200</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+        <v>443590600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24">
-        <v>1610062000</v>
+        <v>848884600</v>
       </c>
       <c r="C24">
-        <v>290786200</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+        <v>411383600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25">
-        <v>1621703100</v>
+        <v>745100500</v>
       </c>
       <c r="C25">
-        <v>352542900</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+        <v>394259900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26">
-        <v>1650243100</v>
+        <v>747000900</v>
       </c>
       <c r="C26">
-        <v>293860100</v>
+        <v>429283700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>767555500</v>
+      </c>
+      <c r="C27">
+        <v>447951800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>802942800</v>
+      </c>
+      <c r="C28">
+        <v>401791700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>784156000</v>
+      </c>
+      <c r="C29">
+        <v>428294600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>743931400</v>
+      </c>
+      <c r="C30">
+        <v>451369300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>743056600</v>
+      </c>
+      <c r="C31">
+        <v>397940700</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>746083600</v>
+      </c>
+      <c r="C32">
+        <v>461733800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>723802300</v>
+      </c>
+      <c r="C33">
+        <v>488389400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>838147700</v>
+      </c>
+      <c r="C34">
+        <v>418248900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>730704100</v>
+      </c>
+      <c r="C35">
+        <v>455616800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>691251900</v>
+      </c>
+      <c r="C36">
+        <v>435630000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>738755200</v>
+      </c>
+      <c r="C37">
+        <v>434301500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>735200100</v>
+      </c>
+      <c r="C38">
+        <v>434327200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>731299200</v>
+      </c>
+      <c r="C39">
+        <v>430997600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>796327200</v>
+      </c>
+      <c r="C40">
+        <v>413162600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>807203700</v>
+      </c>
+      <c r="C41">
+        <v>441068300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>792931500</v>
+      </c>
+      <c r="C42">
+        <v>401396600</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>688916700</v>
+      </c>
+      <c r="C43">
+        <v>438986000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>781577300</v>
+      </c>
+      <c r="C44">
+        <v>392481100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>686473600</v>
+      </c>
+      <c r="C45">
+        <v>422544500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>759783600</v>
+      </c>
+      <c r="C46">
+        <v>417902600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>790698300</v>
+      </c>
+      <c r="C47">
+        <v>390010500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>725308500</v>
+      </c>
+      <c r="C48">
+        <v>404560200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>712449800</v>
+      </c>
+      <c r="C49">
+        <v>461769300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>702079000</v>
+      </c>
+      <c r="C50">
+        <v>434045000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>784383900</v>
+      </c>
+      <c r="C51">
+        <v>465176600</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>